<commit_message>
Update Code for Stats file
</commit_message>
<xml_diff>
--- a/Stats_template.xlsx
+++ b/Stats_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jodisilverman/Repositories/ps1c_d_analytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CA77A4-334E-9248-AAEB-7E95DCF02F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A2441B-6BEA-7B4D-B732-E54D9ED29D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{C3E9E8DF-EFB6-5446-A3D7-8A361C8EF7B3}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="30">
   <si>
     <t>Not Balanced-Review</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Success</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Waystar</t>
   </si>
 </sst>
 </file>
@@ -651,21 +654,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3584E01-6244-2A4A-BA37-51DA5463ABBA}">
-  <dimension ref="C3:L24"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="14" width="1" customWidth="1"/>
+    <col min="4" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="15" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">MID(CELL("filename",B2),FIND("]",CELL("filename",B2))+1,255)</f>
         <v>YYYY-YTD</v>
@@ -691,8 +694,11 @@
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -723,8 +729,11 @@
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -764,8 +773,12 @@
         <f>G5+E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <f>'YYYY-01'!M6+'YYYY-02'!M5+'YYYY-03'!M5+'YYYY-04'!M5+'YYYY-05'!M5+'YYYY-06'!M5+'YYYY-07'!M5+'YYYY-08'!M5+'YYYY-09'!M5+'YYYY-10'!M5+'YYYY-11'!M5+'YYYY-12'!M5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -805,8 +818,12 @@
         <f t="shared" ref="L6:L23" si="4">G6+E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <f>'YYYY-01'!M7+'YYYY-02'!M6+'YYYY-03'!M6+'YYYY-04'!M6+'YYYY-05'!M6+'YYYY-06'!M6+'YYYY-07'!M6+'YYYY-08'!M6+'YYYY-09'!M6+'YYYY-10'!M6+'YYYY-11'!M6+'YYYY-12'!M6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -846,8 +863,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <f>'YYYY-01'!M8+'YYYY-02'!M7+'YYYY-03'!M7+'YYYY-04'!M7+'YYYY-05'!M7+'YYYY-06'!M7+'YYYY-07'!M7+'YYYY-08'!M7+'YYYY-09'!M7+'YYYY-10'!M7+'YYYY-11'!M7+'YYYY-12'!M7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
@@ -887,8 +908,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <f>'YYYY-01'!M10+'YYYY-02'!M8+'YYYY-03'!M8+'YYYY-04'!M8+'YYYY-05'!M8+'YYYY-06'!M8+'YYYY-07'!M8+'YYYY-08'!M8+'YYYY-09'!M8+'YYYY-10'!M8+'YYYY-11'!M8+'YYYY-12'!M8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -928,8 +953,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <f>'YYYY-01'!M11+'YYYY-02'!M9+'YYYY-03'!M9+'YYYY-04'!M9+'YYYY-05'!M9+'YYYY-06'!M9+'YYYY-07'!M9+'YYYY-08'!M9+'YYYY-09'!M9+'YYYY-10'!M9+'YYYY-11'!M9+'YYYY-12'!M9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -969,8 +998,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <f>'YYYY-01'!M12+'YYYY-02'!M10+'YYYY-03'!M10+'YYYY-04'!M10+'YYYY-05'!M10+'YYYY-06'!M10+'YYYY-07'!M10+'YYYY-08'!M10+'YYYY-09'!M10+'YYYY-10'!M10+'YYYY-11'!M10+'YYYY-12'!M10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1010,8 +1043,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <f>'YYYY-01'!M13+'YYYY-02'!M11+'YYYY-03'!M11+'YYYY-04'!M11+'YYYY-05'!M11+'YYYY-06'!M11+'YYYY-07'!M11+'YYYY-08'!M11+'YYYY-09'!M11+'YYYY-10'!M11+'YYYY-11'!M11+'YYYY-12'!M11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1051,8 +1088,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <f>'YYYY-01'!M14+'YYYY-02'!M12+'YYYY-03'!M12+'YYYY-04'!M12+'YYYY-05'!M12+'YYYY-06'!M12+'YYYY-07'!M12+'YYYY-08'!M12+'YYYY-09'!M12+'YYYY-10'!M12+'YYYY-11'!M12+'YYYY-12'!M12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
@@ -1092,8 +1133,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <f>'YYYY-01'!M15+'YYYY-02'!M13+'YYYY-03'!M13+'YYYY-04'!M13+'YYYY-05'!M13+'YYYY-06'!M13+'YYYY-07'!M13+'YYYY-08'!M13+'YYYY-09'!M13+'YYYY-10'!M13+'YYYY-11'!M13+'YYYY-12'!M13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -1133,8 +1178,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <f>'YYYY-01'!M16+'YYYY-02'!M14+'YYYY-03'!M14+'YYYY-04'!M14+'YYYY-05'!M14+'YYYY-06'!M14+'YYYY-07'!M14+'YYYY-08'!M14+'YYYY-09'!M14+'YYYY-10'!M14+'YYYY-11'!M14+'YYYY-12'!M14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1174,8 +1223,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <f>'YYYY-01'!M17+'YYYY-02'!M15+'YYYY-03'!M15+'YYYY-04'!M15+'YYYY-05'!M15+'YYYY-06'!M15+'YYYY-07'!M15+'YYYY-08'!M15+'YYYY-09'!M15+'YYYY-10'!M15+'YYYY-11'!M15+'YYYY-12'!M15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -1215,8 +1268,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <f>'YYYY-01'!M18+'YYYY-02'!M16+'YYYY-03'!M16+'YYYY-04'!M16+'YYYY-05'!M16+'YYYY-06'!M16+'YYYY-07'!M16+'YYYY-08'!M16+'YYYY-09'!M16+'YYYY-10'!M16+'YYYY-11'!M16+'YYYY-12'!M16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -1256,8 +1313,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <f>'YYYY-01'!M19+'YYYY-02'!M17+'YYYY-03'!M17+'YYYY-04'!M17+'YYYY-05'!M17+'YYYY-06'!M17+'YYYY-07'!M17+'YYYY-08'!M17+'YYYY-09'!M17+'YYYY-10'!M17+'YYYY-11'!M17+'YYYY-12'!M17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -1297,8 +1358,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <f>'YYYY-01'!M20+'YYYY-02'!M18+'YYYY-03'!M18+'YYYY-04'!M18+'YYYY-05'!M18+'YYYY-06'!M18+'YYYY-07'!M18+'YYYY-08'!M18+'YYYY-09'!M18+'YYYY-10'!M18+'YYYY-11'!M18+'YYYY-12'!M18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
@@ -1338,8 +1403,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <f>'YYYY-01'!M21+'YYYY-02'!M19+'YYYY-03'!M19+'YYYY-04'!M19+'YYYY-05'!M19+'YYYY-06'!M19+'YYYY-07'!M19+'YYYY-08'!M19+'YYYY-09'!M19+'YYYY-10'!M19+'YYYY-11'!M19+'YYYY-12'!M19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -1379,8 +1448,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <f>'YYYY-01'!M22+'YYYY-02'!M20+'YYYY-03'!M20+'YYYY-04'!M20+'YYYY-05'!M20+'YYYY-06'!M20+'YYYY-07'!M20+'YYYY-08'!M20+'YYYY-09'!M20+'YYYY-10'!M20+'YYYY-11'!M20+'YYYY-12'!M20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
@@ -1420,8 +1493,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <f>'YYYY-01'!M23+'YYYY-02'!M21+'YYYY-03'!M21+'YYYY-04'!M21+'YYYY-05'!M21+'YYYY-06'!M21+'YYYY-07'!M21+'YYYY-08'!M21+'YYYY-09'!M21+'YYYY-10'!M21+'YYYY-11'!M21+'YYYY-12'!M21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
@@ -1461,8 +1538,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <f>'YYYY-01'!M24+'YYYY-02'!M22+'YYYY-03'!M22+'YYYY-04'!M22+'YYYY-05'!M22+'YYYY-06'!M22+'YYYY-07'!M22+'YYYY-08'!M22+'YYYY-09'!M22+'YYYY-10'!M22+'YYYY-11'!M22+'YYYY-12'!M22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
@@ -1502,8 +1583,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <f>'YYYY-01'!M24+'YYYY-02'!M23+'YYYY-03'!M23+'YYYY-04'!M23+'YYYY-05'!M23+'YYYY-06'!M23+'YYYY-07'!M23+'YYYY-08'!M23+'YYYY-09'!M23+'YYYY-10'!M23+'YYYY-11'!M23+'YYYY-12'!M23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="8" t="s">
         <v>22</v>
       </c>
@@ -1540,7 +1625,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="10">
-        <f>IFERROR(#REF!/M24,0)</f>
+        <f>IFERROR((D24+F24)/J24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(M4:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -1556,21 +1645,21 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E42E59E-D61B-1F48-BD57-FF0656015034}">
-  <dimension ref="C3:L24"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="14" width="1" customWidth="1"/>
+    <col min="4" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="15" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">MID(CELL("filename",B2),FIND("]",CELL("filename",B2))+1,255)</f>
         <v>YYYY-09</v>
@@ -1596,8 +1685,11 @@
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -1628,8 +1720,11 @@
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1665,8 +1760,11 @@
         <f>G5+E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1702,8 +1800,11 @@
         <f t="shared" ref="L6:L23" si="4">G6+E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1739,8 +1840,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1776,8 +1880,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1813,8 +1920,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1850,8 +1960,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1887,8 +2000,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1924,8 +2040,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
@@ -1961,8 +2080,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -1998,8 +2120,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -2035,8 +2160,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -2072,8 +2200,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -2109,8 +2240,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -2146,8 +2280,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
@@ -2183,8 +2320,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -2220,8 +2360,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
@@ -2257,8 +2400,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
@@ -2294,8 +2440,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
@@ -2331,8 +2480,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="8" t="s">
         <v>22</v>
       </c>
@@ -2369,7 +2521,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="10">
-        <f>IFERROR(#REF!/M24,0)</f>
+        <f>IFERROR((D24+F24)/J24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(M4:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -2385,21 +2541,21 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81009923-B2B0-B14F-8C17-763137244CAA}">
-  <dimension ref="C3:L24"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="14" width="1" customWidth="1"/>
+    <col min="4" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="15" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">MID(CELL("filename",B2),FIND("]",CELL("filename",B2))+1,255)</f>
         <v>YYYY-10</v>
@@ -2425,8 +2581,11 @@
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -2457,8 +2616,11 @@
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -2494,8 +2656,11 @@
         <f>G5+E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2531,8 +2696,11 @@
         <f t="shared" ref="L6:L23" si="4">G6+E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -2568,8 +2736,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
@@ -2605,8 +2776,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -2642,8 +2816,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -2679,8 +2856,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -2716,8 +2896,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -2753,8 +2936,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
@@ -2790,8 +2976,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -2827,8 +3016,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -2864,8 +3056,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -2901,8 +3096,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -2938,8 +3136,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -2975,8 +3176,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
@@ -3012,8 +3216,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -3049,8 +3256,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
@@ -3086,8 +3296,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
@@ -3123,8 +3336,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
@@ -3160,8 +3376,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="8" t="s">
         <v>22</v>
       </c>
@@ -3198,7 +3417,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="10">
-        <f>IFERROR(#REF!/M24,0)</f>
+        <f>IFERROR((D24+F24)/J24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(M4:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -3214,21 +3437,21 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54DA9B34-1271-0544-9072-E93245094BFD}">
-  <dimension ref="C3:L24"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="14" width="1" customWidth="1"/>
+    <col min="4" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="15" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">MID(CELL("filename",B2),FIND("]",CELL("filename",B2))+1,255)</f>
         <v>YYYY-11</v>
@@ -3254,8 +3477,11 @@
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -3286,8 +3512,11 @@
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -3323,8 +3552,11 @@
         <f>G5+E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -3360,8 +3592,11 @@
         <f t="shared" ref="L6:L23" si="4">G6+E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -3397,8 +3632,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
@@ -3434,8 +3672,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -3471,8 +3712,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -3508,8 +3752,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -3545,8 +3792,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -3582,8 +3832,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
@@ -3619,8 +3872,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -3656,8 +3912,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -3693,8 +3952,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -3730,8 +3992,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -3767,8 +4032,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -3804,8 +4072,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
@@ -3841,8 +4112,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -3878,8 +4152,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
@@ -3915,8 +4192,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
@@ -3952,8 +4232,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
@@ -3989,8 +4272,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="8" t="s">
         <v>22</v>
       </c>
@@ -4027,7 +4313,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="10">
-        <f>IFERROR(#REF!/M24,0)</f>
+        <f>IFERROR((D24+F24)/J24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(M4:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -4043,21 +4333,21 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054D72F9-CA70-5C40-B5CC-730FF796EDEF}">
-  <dimension ref="C3:L24"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="14" width="1" customWidth="1"/>
+    <col min="4" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="15" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">MID(CELL("filename",B2),FIND("]",CELL("filename",B2))+1,255)</f>
         <v>YYYY-12</v>
@@ -4083,8 +4373,11 @@
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -4115,8 +4408,11 @@
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -4152,8 +4448,11 @@
         <f>G5+E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -4189,8 +4488,11 @@
         <f t="shared" ref="L6:L23" si="4">G6+E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -4226,8 +4528,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
@@ -4263,8 +4568,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -4300,8 +4608,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -4337,8 +4648,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -4374,8 +4688,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -4411,8 +4728,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
@@ -4448,8 +4768,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -4485,8 +4808,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -4522,8 +4848,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -4559,8 +4888,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -4596,8 +4928,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -4633,8 +4968,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
@@ -4670,8 +5008,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -4707,8 +5048,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
@@ -4744,8 +5088,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
@@ -4781,8 +5128,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
@@ -4818,8 +5168,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="8" t="s">
         <v>22</v>
       </c>
@@ -4856,7 +5209,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="10">
-        <f>IFERROR(#REF!/M24,0)</f>
+        <f>IFERROR((D24+F24)/J24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(M4:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -4872,21 +5229,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55CE830-43B0-A949-A4F7-6FA7CCEA90DB}">
-  <dimension ref="C3:L24"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="14" width="1" customWidth="1"/>
+    <col min="4" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="15" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">MID(CELL("filename",B2),FIND("]",CELL("filename",B2))+1,255)</f>
         <v>YYYY-01</v>
@@ -4912,8 +5269,11 @@
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -4944,8 +5304,11 @@
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -4981,8 +5344,11 @@
         <f>G5+E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -5018,8 +5384,11 @@
         <f t="shared" ref="L6:L23" si="4">G6+E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -5055,8 +5424,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
@@ -5092,8 +5464,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -5129,8 +5504,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -5166,8 +5544,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -5203,8 +5584,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -5240,8 +5624,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
@@ -5277,8 +5664,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -5314,8 +5704,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -5351,8 +5744,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -5388,8 +5784,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -5425,8 +5824,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -5462,8 +5864,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
@@ -5499,8 +5904,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -5536,8 +5944,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
@@ -5573,8 +5984,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
@@ -5610,8 +6024,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
@@ -5647,8 +6064,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="8" t="s">
         <v>22</v>
       </c>
@@ -5685,7 +6105,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="10">
-        <f>IFERROR(#REF!/M24,0)</f>
+        <f>IFERROR((D24+F24)/J24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(M4:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -5701,21 +6125,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3628CB27-B9C1-3A45-89D1-78906715915A}">
-  <dimension ref="C3:L24"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="14" width="1" customWidth="1"/>
+    <col min="4" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="15" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">MID(CELL("filename",B2),FIND("]",CELL("filename",B2))+1,255)</f>
         <v>YYYY-02</v>
@@ -5741,8 +6165,11 @@
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -5773,8 +6200,11 @@
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -5810,8 +6240,11 @@
         <f>G5+E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -5847,8 +6280,11 @@
         <f t="shared" ref="L6:L23" si="4">G6+E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -5884,8 +6320,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
@@ -5921,8 +6360,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -5958,8 +6400,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -5995,8 +6440,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -6032,8 +6480,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -6069,8 +6520,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
@@ -6106,8 +6560,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -6143,8 +6600,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -6180,8 +6640,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -6217,8 +6680,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -6254,8 +6720,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -6291,8 +6760,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
@@ -6328,8 +6800,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -6365,8 +6840,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
@@ -6402,8 +6880,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
@@ -6439,8 +6920,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
@@ -6476,8 +6960,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="8" t="s">
         <v>22</v>
       </c>
@@ -6514,7 +7001,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="10">
-        <f>IFERROR(#REF!/M24,0)</f>
+        <f>IFERROR((D24+F24)/J24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(M4:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -6530,21 +7021,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB57723-EFDD-0A46-80A5-8813AFCE9E3D}">
-  <dimension ref="C3:L24"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="14" width="1" customWidth="1"/>
+    <col min="4" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="15" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">MID(CELL("filename",B2),FIND("]",CELL("filename",B2))+1,255)</f>
         <v>YYYY-03</v>
@@ -6570,8 +7061,11 @@
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -6602,8 +7096,11 @@
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -6639,8 +7136,11 @@
         <f>G5+E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -6676,8 +7176,11 @@
         <f t="shared" ref="L6:L23" si="4">G6+E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -6713,8 +7216,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
@@ -6750,8 +7256,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -6787,8 +7296,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -6824,8 +7336,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -6861,8 +7376,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -6898,8 +7416,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
@@ -6935,8 +7456,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -6972,8 +7496,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -7009,8 +7536,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -7046,8 +7576,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -7083,8 +7616,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -7120,8 +7656,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
@@ -7157,8 +7696,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -7194,8 +7736,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
@@ -7231,8 +7776,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
@@ -7268,8 +7816,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
@@ -7305,8 +7856,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="8" t="s">
         <v>22</v>
       </c>
@@ -7343,7 +7897,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="10">
-        <f>IFERROR(#REF!/M24,0)</f>
+        <f>IFERROR((D24+F24)/J24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(M4:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -7359,21 +7917,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9680C7-9429-D248-96FB-C962F0053ED4}">
-  <dimension ref="C3:L24"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="14" width="1" customWidth="1"/>
+    <col min="4" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="15" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">MID(CELL("filename",B2),FIND("]",CELL("filename",B2))+1,255)</f>
         <v>YYYY-04</v>
@@ -7399,8 +7957,11 @@
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -7431,8 +7992,11 @@
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -7468,8 +8032,11 @@
         <f>G5+E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -7505,8 +8072,11 @@
         <f t="shared" ref="L6:L23" si="4">G6+E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -7542,8 +8112,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
@@ -7579,8 +8152,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -7616,8 +8192,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -7653,8 +8232,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -7690,8 +8272,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -7727,8 +8312,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
@@ -7764,8 +8352,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -7801,8 +8392,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -7838,8 +8432,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -7875,8 +8472,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -7912,8 +8512,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -7949,8 +8552,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
@@ -7986,8 +8592,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -8023,8 +8632,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
@@ -8060,8 +8672,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
@@ -8097,8 +8712,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
@@ -8134,8 +8752,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="8" t="s">
         <v>22</v>
       </c>
@@ -8172,7 +8793,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="10">
-        <f>IFERROR(#REF!/M24,0)</f>
+        <f>IFERROR((D24+F24)/J24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(M4:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -8188,21 +8813,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7200FE7E-944B-E24A-A4CD-49F09188BCEE}">
-  <dimension ref="C3:L24"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="14" width="1" customWidth="1"/>
+    <col min="4" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="15" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">MID(CELL("filename",B2),FIND("]",CELL("filename",B2))+1,255)</f>
         <v>YYYY-05</v>
@@ -8228,8 +8853,11 @@
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -8260,8 +8888,11 @@
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -8297,8 +8928,11 @@
         <f>G5+E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -8334,8 +8968,11 @@
         <f t="shared" ref="L6:L23" si="4">G6+E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -8371,8 +9008,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
@@ -8408,8 +9048,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -8445,8 +9088,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -8482,8 +9128,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -8519,8 +9168,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -8556,8 +9208,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
@@ -8593,8 +9248,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -8630,8 +9288,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -8667,8 +9328,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -8704,8 +9368,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -8741,8 +9408,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -8778,8 +9448,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
@@ -8815,8 +9488,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -8852,8 +9528,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
@@ -8889,8 +9568,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
@@ -8926,8 +9608,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
@@ -8963,8 +9648,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="8" t="s">
         <v>22</v>
       </c>
@@ -9001,7 +9689,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="10">
-        <f>IFERROR(#REF!/M24,0)</f>
+        <f>IFERROR((D24+F24)/J24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(M4:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -9017,21 +9709,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB5FCDF-F323-CF4C-BE36-DCD87A2C7F70}">
-  <dimension ref="C3:L24"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="14" width="1" customWidth="1"/>
+    <col min="4" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="15" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">MID(CELL("filename",B2),FIND("]",CELL("filename",B2))+1,255)</f>
         <v>YYYY-06</v>
@@ -9057,8 +9749,11 @@
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -9089,8 +9784,11 @@
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -9126,8 +9824,11 @@
         <f>G5+E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -9163,8 +9864,11 @@
         <f t="shared" ref="L6:L23" si="4">G6+E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -9200,8 +9904,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
@@ -9237,8 +9944,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -9274,8 +9984,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -9311,8 +10024,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -9348,8 +10064,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -9385,8 +10104,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
@@ -9422,8 +10144,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -9459,8 +10184,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -9496,8 +10224,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -9533,8 +10264,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -9570,8 +10304,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -9607,8 +10344,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
@@ -9644,8 +10384,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -9681,8 +10424,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
@@ -9718,8 +10464,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
@@ -9755,8 +10504,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
@@ -9792,8 +10544,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="8" t="s">
         <v>22</v>
       </c>
@@ -9830,7 +10585,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="10">
-        <f>IFERROR(#REF!/M24,0)</f>
+        <f>IFERROR((D24+F24)/J24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(M4:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -9846,21 +10605,21 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E182F02F-B190-0940-8C07-B4ECEE720EFC}">
-  <dimension ref="C3:L24"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="14" width="1" customWidth="1"/>
+    <col min="4" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="15" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">MID(CELL("filename",B2),FIND("]",CELL("filename",B2))+1,255)</f>
         <v>YYYY-07</v>
@@ -9886,8 +10645,11 @@
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -9918,8 +10680,11 @@
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -9955,8 +10720,11 @@
         <f>G5+E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -9992,8 +10760,11 @@
         <f t="shared" ref="L6:L23" si="4">G6+E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -10029,8 +10800,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
@@ -10066,8 +10840,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -10103,8 +10880,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -10140,8 +10920,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -10177,8 +10960,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -10214,8 +11000,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
@@ -10251,8 +11040,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -10288,8 +11080,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -10325,8 +11120,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -10362,8 +11160,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -10399,8 +11200,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -10436,8 +11240,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
@@ -10473,8 +11280,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -10510,8 +11320,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
@@ -10547,8 +11360,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
@@ -10584,8 +11400,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
@@ -10621,8 +11440,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="8" t="s">
         <v>22</v>
       </c>
@@ -10659,7 +11481,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="10">
-        <f>IFERROR(#REF!/M24,0)</f>
+        <f>IFERROR((D24+F24)/J24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(M4:M23)</f>
         <v>0</v>
       </c>
     </row>
@@ -10675,21 +11501,21 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF24F998-4609-2B4D-9482-FBE219A174C4}">
-  <dimension ref="C3:L24"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="14" width="1" customWidth="1"/>
+    <col min="4" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="15" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">MID(CELL("filename",B2),FIND("]",CELL("filename",B2))+1,255)</f>
         <v>YYYY-08</v>
@@ -10715,8 +11541,11 @@
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -10747,8 +11576,11 @@
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -10784,8 +11616,11 @@
         <f>G5+E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -10821,8 +11656,11 @@
         <f t="shared" ref="L6:L23" si="4">G6+E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -10858,8 +11696,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
@@ -10895,8 +11736,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -10932,8 +11776,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -10969,8 +11816,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -11006,8 +11856,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
@@ -11043,8 +11896,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
@@ -11080,8 +11936,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -11117,8 +11976,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -11154,8 +12016,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -11191,8 +12056,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -11228,8 +12096,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -11265,8 +12136,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
@@ -11302,8 +12176,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -11339,8 +12216,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
@@ -11376,8 +12256,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
@@ -11413,8 +12296,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
@@ -11450,8 +12336,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="8" t="s">
         <v>22</v>
       </c>
@@ -11488,7 +12377,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="10">
-        <f>IFERROR(#REF!/M24,0)</f>
+        <f>IFERROR((D24+F24)/J24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(M4:M23)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>